<commit_message>
* added exception to constructor that accepts a List<uint> * implemented ToString() * added a throw NotImplementedException on operator-
</commit_message>
<xml_diff>
--- a/BIGNUM/Doc/bugs.xlsx
+++ b/BIGNUM/Doc/bugs.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
   <si>
     <t>Datum rapporterat</t>
   </si>
@@ -73,43 +73,22 @@
     <t>Implementera BigNumber.% (rest vid division) För BigNumber enbart</t>
   </si>
   <si>
-    <t>Implementera MakeEqual, som ser till att storleken på List&lt;uint&gt; _number är lika stor på bägge argumenten. Den största av operanderna får styra. För BigNumber enbart</t>
-  </si>
-  <si>
     <t>Implementera jämförelseoperatorn &gt; För BigNumber enbart</t>
   </si>
   <si>
     <t>Implementera jämförelseoperatorn &lt; För BigNumber enbart</t>
   </si>
   <si>
-    <t>Implementera jämförelseoperatorn = För BigNumber enbart</t>
-  </si>
-  <si>
     <t>Implementera Konstruktorn BigNumber(string)</t>
   </si>
   <si>
     <t>Implementera operator% Rest vid division med ett annat BigNumber. För BigNumber enbart</t>
   </si>
   <si>
-    <t>Implementera jämförelseoperator !</t>
-  </si>
-  <si>
-    <t>Implementera operator &gt;=</t>
-  </si>
-  <si>
-    <t>Implementera operator &lt;=</t>
-  </si>
-  <si>
     <t>Implementera bitwise |, &amp;,  &lt;&lt;, &gt;&gt;,  rotl, rotr, ^</t>
   </si>
   <si>
-    <t>Implementera operator: public Negative som är true om BigNumber är negativt annars false</t>
-  </si>
-  <si>
     <t>Implementera BigNumber.operator+ Obs! För all aritmetik nedan gäller att om resultatet är negativt (-a), lagras (a) samt property Negative = true</t>
-  </si>
-  <si>
-    <t>Implementera BigNumber.operator-. Implementeras med hjälp av en flagga _negative. Let c = a-b . c &lt;  0  =&gt; lagra -(a-b) samt property Negative  = true</t>
   </si>
   <si>
     <t>Implementera överlagrad konstruktor BigNumber(BigNumber num).</t>
@@ -175,12 +154,36 @@
   <si>
     <t>Implementera överlagrad ToString()</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Implementera BigNumber.operator-. Implementeras med hjälp av en flagga _negative. Let c = a-b . c &lt;  0  =&gt; lagra -(a-b) samt property Negative  = true.</t>
+  </si>
+  <si>
+    <t>Implementera jämförelseoperatorn == För BigNumber enbart</t>
+  </si>
+  <si>
+    <t>Implementera jämförelseoperator != För BigNumber enbart</t>
+  </si>
+  <si>
+    <t>Implementera operator &gt;= För BigNumber enbart</t>
+  </si>
+  <si>
+    <t>Implementera operator &lt;= För BigNumber enbart</t>
+  </si>
+  <si>
+    <t>Implementera operator: public Negative som är true om BigNumber är negativt annars false NEGATIVA TAL UTGÅR</t>
+  </si>
+  <si>
+    <t>Implementera MakeEqual, som ser till att storleken på List&lt;uint&gt; _number är lika stor på bägge argumenten. Den största av operanderna får styra. För BigNumber enbart. Utgår. Man kan använda Trim() på de BigNumber som ingår i aritmetiken.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,13 +209,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -297,7 +293,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,8 +598,8 @@
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,7 +651,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -672,7 +668,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -726,7 +722,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -747,22 +743,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="15">
         <v>42981</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="6">
+      <c r="C8" s="15">
+        <v>42986</v>
+      </c>
+      <c r="D8" s="25">
         <v>7</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="25">
         <v>1</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>15</v>
+      <c r="F8" s="17" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -786,43 +784,48 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="15">
         <v>42982</v>
       </c>
-      <c r="C10" s="7">
-        <v>42982</v>
-      </c>
-      <c r="D10" s="6">
+      <c r="C10" s="15">
+        <v>42986</v>
+      </c>
+      <c r="D10" s="25">
         <v>9</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="16">
         <v>2</v>
       </c>
-      <c r="F10" s="9" t="s">
-        <v>25</v>
+      <c r="F10" s="17" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B11" s="4">
         <v>43004</v>
       </c>
-      <c r="C11" s="7"/>
+      <c r="C11" s="7">
+        <v>42986</v>
+      </c>
       <c r="D11" s="2">
         <v>10</v>
       </c>
+      <c r="E11" s="5">
+        <v>2</v>
+      </c>
       <c r="F11" s="11" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B12" s="4">
         <v>43004</v>
@@ -831,14 +834,17 @@
       <c r="D12" s="6">
         <v>11</v>
       </c>
+      <c r="E12" s="8">
+        <v>2</v>
+      </c>
       <c r="F12" s="9" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B13" s="4">
         <v>43004</v>
@@ -847,56 +853,67 @@
       <c r="D13" s="2">
         <v>12</v>
       </c>
+      <c r="E13" s="5">
+        <v>2</v>
+      </c>
       <c r="F13" s="11" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B14" s="7">
         <v>42982</v>
       </c>
-      <c r="C14" s="12"/>
+      <c r="C14" s="7">
+        <v>42986</v>
+      </c>
       <c r="D14" s="6">
         <v>13</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B15" s="7">
         <v>42982</v>
       </c>
-      <c r="C15" s="20"/>
+      <c r="C15" s="7">
+        <v>42986</v>
+      </c>
       <c r="D15" s="2">
         <v>14</v>
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B16" s="7">
         <v>42982</v>
       </c>
-      <c r="C16" s="7"/>
+      <c r="C16" s="7">
+        <v>42986</v>
+      </c>
       <c r="D16" s="6">
         <v>15</v>
       </c>
-      <c r="E16" s="8"/>
+      <c r="E16" s="8">
+        <v>2</v>
+      </c>
       <c r="F16" s="9" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -906,7 +923,7 @@
       <c r="B17" s="7">
         <v>42983</v>
       </c>
-      <c r="C17" s="25">
+      <c r="C17" s="12">
         <v>42984</v>
       </c>
       <c r="D17" s="2">
@@ -916,7 +933,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -930,9 +947,11 @@
       <c r="D18" s="6">
         <v>17</v>
       </c>
-      <c r="E18" s="8"/>
+      <c r="E18" s="8">
+        <v>1</v>
+      </c>
       <c r="F18" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -948,7 +967,7 @@
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -963,7 +982,7 @@
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="11" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -979,7 +998,7 @@
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="11" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -996,7 +1015,7 @@
         <v>2</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1016,7 +1035,7 @@
         <v>3</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1026,7 +1045,9 @@
       <c r="B24" s="7">
         <v>42986</v>
       </c>
-      <c r="C24" s="7"/>
+      <c r="C24" s="7">
+        <v>42986</v>
+      </c>
       <c r="D24" s="2">
         <v>24</v>
       </c>
@@ -1034,10 +1055,13 @@
         <v>1</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="D25" s="6">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
* BigNumber: reintroduced flag IsNegative * BigNumber: introduced regions for clarity * BigNumber: now throws an exception if the object has no data to trim * BigNumber: operator now does -(b -a) if (a < b) * BigNumber: minor bugfix - there stood < on two places where it should have been <= * BigNumber: added operator >= and operator <= * Bugs.xls: filled in actions taken * Main.cs: changed what is being tested right now
</commit_message>
<xml_diff>
--- a/BIGNUM/Doc/bugs.xlsx
+++ b/BIGNUM/Doc/bugs.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Buggar!$A$1:$G$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Buggar!$A$1:$G$102</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>Datum rapporterat</t>
   </si>
@@ -158,9 +158,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Implementera BigNumber.operator-. Implementeras med hjälp av en flagga _negative. Let c = a-b . c &lt;  0  =&gt; lagra -(a-b) samt property Negative  = true.</t>
-  </si>
-  <si>
     <t>Implementera jämförelseoperatorn == För BigNumber enbart</t>
   </si>
   <si>
@@ -173,10 +170,25 @@
     <t>Implementera operator &lt;= För BigNumber enbart</t>
   </si>
   <si>
-    <t>Implementera operator: public Negative som är true om BigNumber är negativt annars false NEGATIVA TAL UTGÅR</t>
-  </si>
-  <si>
-    <t>Implementera MakeEqual, som ser till att storleken på List&lt;uint&gt; _number är lika stor på bägge argumenten. Den största av operanderna får styra. För BigNumber enbart. Utgår. Man kan använda Trim() på de BigNumber som ingår i aritmetiken.</t>
+    <t>0.1.2.0</t>
+  </si>
+  <si>
+    <t>0.2.0.0</t>
+  </si>
+  <si>
+    <t>Implementera BigNumber.operator-. Unärt minus. Implementeras med hjälp av en flagga _negative. Let c = a-b . c &lt;  0  =&gt; lagra -(a-b) samt property Negative  = true.</t>
+  </si>
+  <si>
+    <t>Implementera MakeEqual, som ser till att storleken på List&lt;uint&gt; _number är lika stor på bägge argumenten. Den största av operanderna får styra. För BigNumber enbart. Utgår. Man kan använda Trim() på de BigNumber som ingår i aritmetiken.Utgår eftersom numren har skapats via konstruktorer,  och då har de trimmats.</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Implementera operator: public Negative som är true om BigNumber är negativt annars false</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -249,51 +261,78 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,906 +634,944 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G100"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="22" customWidth="1"/>
-    <col min="2" max="3" width="14.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="20" customWidth="1"/>
+    <col min="2" max="3" width="14.7109375" style="15" customWidth="1"/>
     <col min="4" max="4" width="7.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="163.85546875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="163.85546875" style="25" customWidth="1"/>
     <col min="7" max="7" width="54.7109375" customWidth="1"/>
     <col min="8" max="8" width="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="14">
         <v>42981</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="6">
+      <c r="C2" s="15">
+        <v>42987</v>
+      </c>
+      <c r="D2" s="3">
         <v>1</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="3">
         <v>1</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="23" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="14">
         <v>42981</v>
       </c>
-      <c r="D3" s="6">
+      <c r="C3" s="15">
+        <v>42987</v>
+      </c>
+      <c r="D3" s="3">
         <v>2</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="3">
         <v>1</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>28</v>
+      <c r="F3" s="23" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="14">
         <v>42981</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="6">
+      <c r="C4" s="14"/>
+      <c r="D4" s="3">
         <v>3</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="3">
         <v>1</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="14">
+        <v>42981</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="3">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="14">
+        <v>42981</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="3">
+        <v>5</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="14">
+        <v>42981</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="3">
+        <v>6</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B8" s="16">
         <v>42981</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="6">
-        <v>4</v>
-      </c>
-      <c r="E5" s="6">
+      <c r="C8" s="16">
+        <v>42986</v>
+      </c>
+      <c r="D8" s="5">
+        <v>7</v>
+      </c>
+      <c r="E8" s="5">
         <v>1</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="7">
+      <c r="F8" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="14">
         <v>42981</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="6">
+      <c r="C9" s="14">
+        <v>42981</v>
+      </c>
+      <c r="D9" s="3">
+        <v>8</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="6">
+      <c r="B10" s="14">
+        <v>42982</v>
+      </c>
+      <c r="C10" s="14">
+        <v>42986</v>
+      </c>
+      <c r="D10" s="3">
+        <v>9</v>
+      </c>
+      <c r="E10" s="3">
         <v>2</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="7">
-        <v>42981</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="6">
-        <v>6</v>
-      </c>
-      <c r="E7" s="6">
-        <v>2</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="15">
-        <v>42981</v>
-      </c>
-      <c r="C8" s="15">
-        <v>42986</v>
-      </c>
-      <c r="D8" s="25">
-        <v>7</v>
-      </c>
-      <c r="E8" s="25">
-        <v>1</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="F10" s="23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="7">
-        <v>42981</v>
-      </c>
-      <c r="C9" s="7">
-        <v>42981</v>
-      </c>
-      <c r="D9" s="6">
-        <v>8</v>
-      </c>
-      <c r="E9" s="8">
-        <v>2</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="15">
-        <v>42982</v>
-      </c>
-      <c r="C10" s="15">
-        <v>42986</v>
-      </c>
-      <c r="D10" s="25">
-        <v>9</v>
-      </c>
-      <c r="E10" s="16">
-        <v>2</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="4">
-        <v>43004</v>
-      </c>
-      <c r="C11" s="7">
+      <c r="B11" s="15">
+        <v>42984</v>
+      </c>
+      <c r="C11" s="14">
         <v>42986</v>
       </c>
       <c r="D11" s="2">
         <v>10</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="2">
         <v>2</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="15">
+        <v>42984</v>
+      </c>
+      <c r="C12" s="14">
+        <v>42986</v>
+      </c>
+      <c r="D12" s="3">
+        <v>11</v>
+      </c>
+      <c r="E12" s="3">
+        <v>2</v>
+      </c>
+      <c r="F12" s="23" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="4">
-        <v>43004</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="6">
-        <v>11</v>
-      </c>
-      <c r="E12" s="8">
-        <v>2</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="20"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="4">
-        <v>43004</v>
-      </c>
-      <c r="C13" s="7"/>
+      <c r="B13" s="15">
+        <v>42984</v>
+      </c>
+      <c r="C13" s="14">
+        <v>42986</v>
+      </c>
       <c r="D13" s="2">
         <v>12</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="2">
         <v>2</v>
       </c>
-      <c r="F13" s="11" t="s">
-        <v>32</v>
+      <c r="F13" s="25" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="14">
         <v>42982</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="14">
         <v>42986</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="3">
         <v>13</v>
       </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="14" t="s">
+      <c r="E14" s="6">
+        <v>2</v>
+      </c>
+      <c r="F14" s="26" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="14">
         <v>42982</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="14">
         <v>42986</v>
       </c>
       <c r="D15" s="2">
         <v>14</v>
       </c>
-      <c r="E15" s="20"/>
-      <c r="F15" s="14" t="s">
+      <c r="E15" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="26" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="14">
         <v>42982</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="14">
         <v>42986</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="3">
         <v>15</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="3">
         <v>2</v>
       </c>
-      <c r="F16" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
+      <c r="F16" s="23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="14">
         <v>42983</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="17">
         <v>42984</v>
       </c>
       <c r="D17" s="2">
         <v>16</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="2">
         <v>1</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="25" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+    <row r="18" spans="1:6" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="15">
         <v>42984</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="6">
+      <c r="C18" s="14"/>
+      <c r="D18" s="3">
         <v>17</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="3">
         <v>1</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="15">
         <v>42984</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="6">
+      <c r="C19" s="14"/>
+      <c r="D19" s="3">
         <v>19</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="9" t="s">
+      <c r="E19" s="3"/>
+      <c r="F19" s="23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="15">
         <v>42984</v>
       </c>
       <c r="D20" s="2">
         <v>20</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="11" t="s">
+      <c r="E20" s="3"/>
+      <c r="F20" s="25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="15">
         <v>42984</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="6">
+      <c r="C21" s="14"/>
+      <c r="D21" s="3">
         <v>21</v>
       </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="11" t="s">
+      <c r="E21" s="3"/>
+      <c r="F21" s="25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="15">
         <v>42985</v>
       </c>
       <c r="D22" s="2">
         <v>22</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="2">
         <v>2</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="25" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="15">
         <v>42985</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="14">
         <v>42986</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="3">
         <v>23</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="3">
         <v>3</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="F23" s="23" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="14">
         <v>42986</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="14">
         <v>42986</v>
       </c>
       <c r="D24" s="2">
         <v>24</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="3">
         <v>1</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="F24" s="23" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C25" s="4" t="s">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="15">
+        <v>42986</v>
+      </c>
+      <c r="C25" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
+      <c r="E25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="19"/>
       <c r="D26" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="6">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="19"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="3">
         <v>27</v>
       </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="14"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="26"/>
+    </row>
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="19"/>
       <c r="D28" s="2">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
-      <c r="D29" s="6">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="19"/>
+      <c r="D29" s="3">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="19"/>
       <c r="D30" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
-      <c r="D31" s="6">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="19"/>
+      <c r="D31" s="3">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="19"/>
       <c r="D32" s="2">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
-      <c r="D33" s="6">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="19"/>
+      <c r="D33" s="3">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="19"/>
       <c r="D34" s="2">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
-      <c r="D35" s="6">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="19"/>
+      <c r="D35" s="3">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="19"/>
       <c r="D36" s="2">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
-      <c r="D37" s="6">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="19"/>
+      <c r="D37" s="3">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="20"/>
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="19"/>
       <c r="D38" s="2">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="20"/>
-      <c r="D39" s="6">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="19"/>
+      <c r="D39" s="3">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="20"/>
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="19"/>
       <c r="D40" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="21"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="6">
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="3">
         <v>41</v>
       </c>
-      <c r="E41" s="16"/>
-      <c r="F41" s="17"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="20"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="24"/>
+    </row>
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="19"/>
       <c r="D42" s="2">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
-      <c r="D43" s="6">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="19"/>
+      <c r="D43" s="3">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="20"/>
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="19"/>
       <c r="D44" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
-      <c r="D45" s="6">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="19"/>
+      <c r="D45" s="3">
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="20"/>
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="19"/>
       <c r="D46" s="2">
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="20"/>
-      <c r="D47" s="6">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="19"/>
+      <c r="D47" s="3">
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="20"/>
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="19"/>
       <c r="D48" s="2">
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="20"/>
-      <c r="D49" s="6">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="19"/>
+      <c r="D49" s="3">
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="20"/>
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="19"/>
       <c r="D50" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="20"/>
-      <c r="D51" s="6">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="19"/>
+      <c r="D51" s="3">
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="20"/>
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="19"/>
       <c r="D52" s="2">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="20"/>
-      <c r="B53" s="7"/>
-      <c r="D53" s="6">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="19"/>
+      <c r="B53" s="14"/>
+      <c r="D53" s="3">
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="20"/>
-      <c r="B54" s="7"/>
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="19"/>
+      <c r="B54" s="14"/>
       <c r="D54" s="2">
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="6">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="3">
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D56" s="2">
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D57" s="6">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D57" s="3">
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D58" s="2">
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D59" s="6">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D59" s="3">
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D60" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D61" s="6">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D61" s="3">
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D62" s="2">
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D63" s="6">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D63" s="3">
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D64" s="2">
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D65" s="6">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D65" s="3">
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D66" s="2">
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D67" s="6">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D67" s="3">
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D68" s="2">
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D69" s="6">
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D69" s="3">
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="21"/>
-      <c r="B70" s="15"/>
-      <c r="C70" s="15"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="16"/>
       <c r="D70" s="2">
         <v>70</v>
       </c>
-      <c r="E70" s="16"/>
-      <c r="F70" s="17"/>
-      <c r="G70" s="23"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D71" s="6">
+      <c r="E70" s="5"/>
+      <c r="F70" s="24"/>
+      <c r="G70" s="8"/>
+    </row>
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D71" s="3">
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D72" s="2">
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D73" s="6">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D73" s="3">
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D74" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D75" s="6">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D75" s="3">
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D76" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D77" s="6">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D77" s="3">
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D78" s="2">
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D79" s="6">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D79" s="3">
         <v>79</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="21"/>
-      <c r="B80" s="15"/>
-      <c r="C80" s="15"/>
+      <c r="B80" s="16"/>
+      <c r="C80" s="16"/>
       <c r="D80" s="2">
         <v>80</v>
       </c>
-      <c r="E80" s="16"/>
-      <c r="F80" s="17"/>
-    </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D81" s="6">
+      <c r="E80" s="5"/>
+      <c r="F80" s="24"/>
+    </row>
+    <row r="81" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D81" s="3">
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D82" s="2">
         <v>82</v>
       </c>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D83" s="6">
+    <row r="83" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D83" s="3">
         <v>83</v>
       </c>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D84" s="2">
         <v>84</v>
       </c>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D85" s="6">
+    <row r="85" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D85" s="3">
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D86" s="2">
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D87" s="6">
+    <row r="87" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D87" s="3">
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D88" s="2">
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D89" s="6">
+    <row r="89" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D89" s="3">
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D90" s="2">
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D91" s="6">
+    <row r="91" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D91" s="3">
         <v>91</v>
       </c>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D92" s="2">
         <v>92</v>
       </c>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D93" s="6">
+    <row r="93" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D93" s="3">
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D94" s="2">
         <v>94</v>
       </c>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D95" s="6">
+    <row r="95" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D95" s="3">
         <v>95</v>
       </c>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D96" s="2">
         <v>96</v>
       </c>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D97" s="6">
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D97" s="3">
         <v>97</v>
       </c>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D98" s="2">
         <v>98</v>
       </c>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D99" s="6">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D99" s="3">
         <v>99</v>
       </c>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D100" s="2">
         <v>100</v>
       </c>
     </row>
+    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B102" s="15">
+        <v>42986</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G101"/>
+  <autoFilter ref="A1:G102">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="0.1.0.0"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1518,16 +1595,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C2" s="4"/>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C3" s="4"/>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C4" s="4"/>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C5" s="4"/>
+      <c r="C5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
* BigNumber: implemented operator* * BigNumber: implemented implicit operator BigNumber(string), which allows the user to assign a text string to a BigNumber * BigNumber: bugfix in operator< -had accidentally used "<" instead of ">" inside the for-loop * BigNumber: region "Operators" was renamed "Comparison operators" for clarity * BigNumber: added constructor BigNumber(ulong num) * BigNumber: changed output between items from D10 to D0 * BigNumber: changed BASE to 10 when we are developing * BigNumber: tested changing back to (uint)0xFFFFFFFF to see what happened to assignment to an integer string. The effect was the same, one digit per slot in the list.
</commit_message>
<xml_diff>
--- a/BIGNUM/Doc/bugs.xlsx
+++ b/BIGNUM/Doc/bugs.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Buggar!$A$1:$G$102</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Buggar!$A$1:$G$104</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
   <si>
     <t>Datum rapporterat</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Implementera BigNumber.operator/ För BigNumber enbart</t>
   </si>
   <si>
-    <t>Implementera BigNumber.% (rest vid division) För BigNumber enbart</t>
-  </si>
-  <si>
     <t>Implementera jämförelseoperatorn &gt; För BigNumber enbart</t>
   </si>
   <si>
@@ -82,9 +79,6 @@
     <t>Implementera Konstruktorn BigNumber(string)</t>
   </si>
   <si>
-    <t>Implementera operator% Rest vid division med ett annat BigNumber. För BigNumber enbart</t>
-  </si>
-  <si>
     <t>Implementera bitwise |, &amp;,  &lt;&lt;, &gt;&gt;,  rotl, rotr, ^</t>
   </si>
   <si>
@@ -95,12 +89,6 @@
   </si>
   <si>
     <t>Implementera BigNumber.operator^ Bitwise XOR. För BigNumber enbart</t>
-  </si>
-  <si>
-    <t>Implementera operator -- . Både post- och predekrement</t>
-  </si>
-  <si>
-    <t>Implementera operator ++ . Både post- och preinkrement</t>
   </si>
   <si>
     <r>
@@ -155,9 +143,6 @@
     <t>Implementera överlagrad ToString()</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Implementera jämförelseoperatorn == För BigNumber enbart</t>
   </si>
   <si>
@@ -170,12 +155,6 @@
     <t>Implementera operator &lt;= För BigNumber enbart</t>
   </si>
   <si>
-    <t>0.1.2.0</t>
-  </si>
-  <si>
-    <t>0.2.0.0</t>
-  </si>
-  <si>
     <t>Implementera BigNumber.operator-. Unärt minus. Implementeras med hjälp av en flagga _negative. Let c = a-b . c &lt;  0  =&gt; lagra -(a-b) samt property Negative  = true.</t>
   </si>
   <si>
@@ -189,6 +168,39 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>Implementera operator* För BigNumber enbart</t>
+  </si>
+  <si>
+    <t>Implementera BigNumber.operator% (rest vid division) För BigNumber enbart</t>
+  </si>
+  <si>
+    <t>Fel i additionen. rad 251 "val -= HALFWORDMAX"  - det bör stå något annat där istället om val är större än BASE</t>
+  </si>
+  <si>
+    <t>Implementera operator ++ . Både post- och preinkrement. Kompilatorn lägger själv ut kod för post- respektive pre-inkrement, så det behöver bara implementeras operator++.</t>
+  </si>
+  <si>
+    <t>Implementera operator -- . Se post 20 för förklaring varför endast en operator kan implementeras.</t>
+  </si>
+  <si>
+    <t>0.1.0.4</t>
+  </si>
+  <si>
+    <t>Testa all implementerad funktionalitet GRUNDLIGT.</t>
+  </si>
+  <si>
+    <t>Gör en funktion Compress(), som ser till att utnyttja HALFWORDMAX till det yttersta. Tanken är om man har använt konstruktorn med en bas 10-sträng, så lagras en siffra per element i listan, vilket är slöseri med utrymme.</t>
+  </si>
+  <si>
+    <t>Göra reverse på ett tal, dvs om LSB-ordet är 1, nästa är 5 och sista är 4 skall resultatet bli att LSB-ordet blir 4, nästa 5 och sista 1. Motivet???</t>
+  </si>
+  <si>
+    <t>Implementerade en implicit operator BigNumber(string) så att man nu kan tilldela ett BigNumber ett strängvärde, och därmed instantiera BigNumber med BigNumber(num). Kunde inte avhålla mig, då det saknas möjlighet till överlagring av operator=</t>
+  </si>
+  <si>
+    <t>Hårdoptimera för hastighet. Förallokera t.ex. listor om man vet deras storlek på förhand.</t>
   </si>
 </sst>
 </file>
@@ -634,12 +646,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:G102"/>
+  <dimension ref="A1:G104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,7 +704,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -713,7 +724,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -734,7 +745,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>11</v>
       </c>
@@ -745,14 +756,14 @@
       <c r="D5" s="3">
         <v>4</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>36</v>
+      <c r="E5" s="3">
+        <v>1</v>
       </c>
       <c r="F5" s="23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>11</v>
       </c>
@@ -767,10 +778,10 @@
         <v>2</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>11</v>
       </c>
@@ -782,13 +793,13 @@
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>7</v>
       </c>
@@ -805,7 +816,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -845,7 +856,7 @@
         <v>2</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -865,7 +876,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -885,7 +896,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G12" s="7"/>
     </row>
@@ -906,7 +917,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -926,7 +937,7 @@
         <v>2</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -943,10 +954,10 @@
         <v>14</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -966,7 +977,7 @@
         <v>2</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -986,17 +997,19 @@
         <v>1</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="15">
         <v>42984</v>
       </c>
-      <c r="C18" s="14"/>
+      <c r="C18" s="15">
+        <v>42988</v>
+      </c>
       <c r="D18" s="3">
         <v>17</v>
       </c>
@@ -1004,574 +1017,640 @@
         <v>1</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" s="15">
         <v>42984</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="3">
-        <v>19</v>
-      </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="23" t="s">
+      <c r="C19" s="14">
+        <v>42986</v>
+      </c>
+      <c r="D19" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" s="15">
         <v>42984</v>
       </c>
-      <c r="D20" s="2">
+      <c r="C20" s="14">
+        <v>42986</v>
+      </c>
+      <c r="D20" s="3">
+        <v>19</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1</v>
+      </c>
+      <c r="F20" s="25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="15">
+        <v>42985</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="2">
         <v>20</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="15">
-        <v>42984</v>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="3">
-        <v>21</v>
-      </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="2">
+        <v>2</v>
+      </c>
       <c r="F21" s="25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
+        <v>5</v>
       </c>
       <c r="B22" s="15">
         <v>42985</v>
       </c>
-      <c r="D22" s="2">
-        <v>22</v>
-      </c>
-      <c r="E22" s="2">
-        <v>2</v>
-      </c>
-      <c r="F22" s="25" t="s">
-        <v>19</v>
+      <c r="C22" s="14">
+        <v>42986</v>
+      </c>
+      <c r="D22" s="3">
+        <v>21</v>
+      </c>
+      <c r="E22" s="3">
+        <v>3</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="15">
-        <v>42985</v>
+      <c r="B23" s="14">
+        <v>42986</v>
       </c>
       <c r="C23" s="14">
         <v>42986</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
+        <v>22</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="15">
+        <v>42986</v>
+      </c>
+      <c r="C24" s="17">
+        <v>42988</v>
+      </c>
+      <c r="D24" s="3">
         <v>23</v>
       </c>
-      <c r="E23" s="3">
-        <v>3</v>
-      </c>
-      <c r="F23" s="23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="14">
-        <v>42986</v>
-      </c>
-      <c r="C24" s="14">
-        <v>42986</v>
-      </c>
-      <c r="D24" s="2">
-        <v>24</v>
-      </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <v>1</v>
       </c>
-      <c r="F24" s="23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="B25" s="15">
         <v>42986</v>
       </c>
-      <c r="C25" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="3">
-        <v>25</v>
+      <c r="C25" s="15">
+        <v>42986</v>
+      </c>
+      <c r="D25" s="2">
+        <v>24</v>
       </c>
       <c r="E25" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
-      <c r="D26" s="2">
+      <c r="F25" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="17">
+        <v>42988</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="3">
+        <v>25</v>
+      </c>
+      <c r="E26" s="6">
+        <v>3</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="15">
+        <v>42987</v>
+      </c>
+      <c r="C27" s="15">
+        <v>42987</v>
+      </c>
+      <c r="D27" s="2">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="3">
+      <c r="E27" s="2">
+        <v>2</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="15">
+        <v>42988</v>
+      </c>
+      <c r="D28" s="3">
         <v>27</v>
       </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="26"/>
-    </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
-      <c r="D28" s="2">
+      <c r="E28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="15">
+        <v>42988</v>
+      </c>
+      <c r="D29" s="2">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
-      <c r="D29" s="3">
+      <c r="E29" s="2">
+        <v>1</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="15">
+        <v>42988</v>
+      </c>
+      <c r="D30" s="3">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
-      <c r="D30" s="2">
+      <c r="F30" s="25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="19"/>
+      <c r="D31" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
-      <c r="D31" s="3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="19"/>
+      <c r="D32" s="3">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
-      <c r="D32" s="2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="19"/>
+      <c r="D33" s="2">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
-      <c r="D33" s="3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="19"/>
+      <c r="D34" s="3">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
-      <c r="D34" s="2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="19"/>
+      <c r="D35" s="2">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="19"/>
-      <c r="D35" s="3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="19"/>
+      <c r="D36" s="3">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
-      <c r="D36" s="2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="19"/>
+      <c r="D37" s="2">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
-      <c r="D37" s="3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="19"/>
+      <c r="D38" s="3">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
-      <c r="D38" s="2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="19"/>
+      <c r="D39" s="2">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
-      <c r="D39" s="3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="21"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="3">
         <v>39</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
-      <c r="D40" s="2">
+      <c r="E40" s="5"/>
+      <c r="F40" s="24"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="19"/>
+      <c r="D41" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="19"/>
+      <c r="D42" s="3">
         <v>41</v>
       </c>
-      <c r="E41" s="5"/>
-      <c r="F41" s="24"/>
-    </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="19"/>
-      <c r="D42" s="2">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="19"/>
+      <c r="D43" s="2">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="19"/>
-      <c r="D43" s="3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="19"/>
+      <c r="D44" s="3">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="19"/>
-      <c r="D44" s="2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="19"/>
+      <c r="D45" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="19"/>
-      <c r="D45" s="3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="19"/>
+      <c r="D46" s="3">
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="19"/>
-      <c r="D46" s="2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="19"/>
+      <c r="D47" s="2">
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="19"/>
-      <c r="D47" s="3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="19"/>
+      <c r="D48" s="3">
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="19"/>
-      <c r="D48" s="2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="19"/>
+      <c r="D49" s="2">
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="19"/>
-      <c r="D49" s="3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="19"/>
+      <c r="D50" s="3">
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="19"/>
-      <c r="D50" s="2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="19"/>
+      <c r="D51" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="19"/>
-      <c r="D51" s="3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="19"/>
+      <c r="B52" s="14"/>
+      <c r="D52" s="3">
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="19"/>
-      <c r="D52" s="2">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="19"/>
       <c r="B53" s="14"/>
-      <c r="D53" s="3">
+      <c r="D53" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="3">
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="19"/>
-      <c r="B54" s="14"/>
-      <c r="D54" s="2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="2">
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="3">
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D56" s="2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="2">
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D57" s="3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="3">
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D58" s="2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="2">
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D59" s="3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="3">
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D60" s="2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D61" s="3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="3">
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D62" s="2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="2">
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D63" s="3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D64" s="3">
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D64" s="2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D65" s="2">
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D65" s="3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D66" s="3">
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D66" s="2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D67" s="2">
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D67" s="3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D68" s="3">
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D68" s="2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="21"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="16"/>
+      <c r="D69" s="2">
         <v>68</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D69" s="3">
+      <c r="E69" s="5"/>
+      <c r="F69" s="24"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D70" s="3">
         <v>69</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="21"/>
-      <c r="B70" s="16"/>
-      <c r="C70" s="16"/>
-      <c r="D70" s="2">
+      <c r="G70" s="8"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D71" s="2">
         <v>70</v>
       </c>
-      <c r="E70" s="5"/>
-      <c r="F70" s="24"/>
-      <c r="G70" s="8"/>
-    </row>
-    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D71" s="3">
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D72" s="3">
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D72" s="2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D73" s="2">
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D73" s="3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D74" s="3">
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D74" s="2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D75" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D75" s="3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D76" s="3">
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D76" s="2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D77" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D77" s="3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D78" s="3">
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D78" s="2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="21"/>
+      <c r="B79" s="16"/>
+      <c r="C79" s="16"/>
+      <c r="D79" s="2">
         <v>78</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D79" s="3">
+      <c r="E79" s="5"/>
+      <c r="F79" s="24"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D80" s="3">
         <v>79</v>
       </c>
     </row>
-    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="21"/>
-      <c r="B80" s="16"/>
-      <c r="C80" s="16"/>
-      <c r="D80" s="2">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" s="2">
         <v>80</v>
       </c>
-      <c r="E80" s="5"/>
-      <c r="F80" s="24"/>
-    </row>
-    <row r="81" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D81" s="3">
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D82" s="3">
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D82" s="2">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="2">
         <v>82</v>
       </c>
     </row>
-    <row r="83" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D83" s="3">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="3">
         <v>83</v>
       </c>
     </row>
-    <row r="84" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D84" s="2">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D85" s="2">
         <v>84</v>
       </c>
     </row>
-    <row r="85" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D85" s="3">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D86" s="3">
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D86" s="2">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D87" s="2">
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D87" s="3">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D88" s="3">
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D88" s="2">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D89" s="2">
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D89" s="3">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D90" s="3">
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D90" s="2">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D91" s="2">
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D91" s="3">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D92" s="3">
         <v>91</v>
       </c>
     </row>
-    <row r="92" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D92" s="2">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D93" s="2">
         <v>92</v>
       </c>
     </row>
-    <row r="93" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D93" s="3">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D94" s="3">
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D94" s="2">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D95" s="2">
         <v>94</v>
       </c>
     </row>
-    <row r="95" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D95" s="3">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D96" s="3">
         <v>95</v>
       </c>
     </row>
-    <row r="96" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D96" s="2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D97" s="2">
         <v>96</v>
       </c>
     </row>
-    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D97" s="3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D98" s="3">
         <v>97</v>
       </c>
     </row>
-    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D98" s="2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D99" s="2">
         <v>98</v>
       </c>
     </row>
-    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D99" s="3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D100" s="3">
         <v>99</v>
       </c>
     </row>
-    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D100" s="2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D101" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B102" s="15">
-        <v>42986</v>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B104" s="15">
+        <v>42988</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G102">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="0.1.0.0"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G104"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Bugfix to function Trim(). Now it creates at least one element in the internal _number data structure. A lot of functions depend on it.
</commit_message>
<xml_diff>
--- a/BIGNUM/Doc/bugs.xlsx
+++ b/BIGNUM/Doc/bugs.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Buggar!$A$1:$G$104</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Buggar!$A$1:$G$106</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
   <si>
     <t>Datum rapporterat</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>Implementera Konstruktorn BigNumber(string)</t>
-  </si>
-  <si>
-    <t>Implementera bitwise |, &amp;,  &lt;&lt;, &gt;&gt;,  rotl, rotr, ^</t>
   </si>
   <si>
     <t>Implementera BigNumber.operator+ Obs! För all aritmetik nedan gäller att om resultatet är negativt (-a), lagras (a) samt property Negative = true</t>
@@ -201,6 +198,63 @@
   </si>
   <si>
     <t>Hårdoptimera för hastighet. Förallokera t.ex. listor om man vet deras storlek på förhand.</t>
+  </si>
+  <si>
+    <t>Korrigera datat från bas 10-strängarna till BASE-basen (dvs. den som inte var satt till 10 under testerna). Se BigNumber(string).</t>
+  </si>
+  <si>
+    <t>Gå igenom alla Exceptions och kolla att rätt exception kastas vid rätt tillf älle</t>
+  </si>
+  <si>
+    <t>Implementera funktionen EXP, som gör lhs upphöjt till rhs.</t>
+  </si>
+  <si>
+    <t>Implmentera MODEXP, som gör moduloexponentierieng med optimering, dvs ej lhs**rhs MOD p utan använder sig av algoritmer som jag har implementerat i CLongBin.CPP</t>
+  </si>
+  <si>
+    <t>Implementera bitwise &amp;</t>
+  </si>
+  <si>
+    <t>Implementera bitwise «</t>
+  </si>
+  <si>
+    <t>Implementera bitwise »</t>
+  </si>
+  <si>
+    <t>Implementera bitwise rotl</t>
+  </si>
+  <si>
+    <t>Implementera bitwise rotr</t>
+  </si>
+  <si>
+    <t>Implementera bitwise ^ (XOR)</t>
+  </si>
+  <si>
+    <r>
+      <t>Implementera bitwise |, &amp;,  &lt;&lt;, &gt;&gt;,  rotl, rotr, ^</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Har splittrat upp aktiviteterna en för en.</t>
+    </r>
+  </si>
+  <si>
+    <t>Implementera /=</t>
+  </si>
+  <si>
+    <t>Implementera *=</t>
+  </si>
+  <si>
+    <t>Implementera -=</t>
+  </si>
+  <si>
+    <t>Implementera +=</t>
   </si>
 </sst>
 </file>
@@ -646,11 +700,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G104"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +758,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -724,7 +778,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -765,7 +819,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" s="14">
         <v>42981</v>
@@ -778,7 +832,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -793,10 +847,10 @@
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -816,7 +870,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -856,7 +910,7 @@
         <v>2</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -876,7 +930,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -896,7 +950,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G12" s="7"/>
     </row>
@@ -917,7 +971,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -954,7 +1008,7 @@
         <v>14</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F15" s="26" t="s">
         <v>15</v>
@@ -977,7 +1031,7 @@
         <v>2</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -997,7 +1051,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1037,7 +1091,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1057,25 +1111,25 @@
         <v>1</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="15">
+      <c r="A21" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="16">
         <v>42985</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="2">
+      <c r="C21" s="16"/>
+      <c r="D21" s="5">
         <v>20</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="5">
         <v>2</v>
       </c>
-      <c r="F21" s="25" t="s">
-        <v>17</v>
+      <c r="F21" s="24" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1095,7 +1149,7 @@
         <v>3</v>
       </c>
       <c r="F22" s="23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1115,7 +1169,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1135,7 +1189,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1155,12 +1209,12 @@
         <v>1</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="17">
         <v>42988</v>
@@ -1173,7 +1227,7 @@
         <v>3</v>
       </c>
       <c r="F26" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1193,12 +1247,12 @@
         <v>2</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B28" s="15">
         <v>42988</v>
@@ -1207,10 +1261,10 @@
         <v>27</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1223,16 +1277,16 @@
       <c r="D29" s="2">
         <v>28</v>
       </c>
-      <c r="E29" s="2">
-        <v>1</v>
+      <c r="E29" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="15">
         <v>42988</v>
@@ -1240,417 +1294,575 @@
       <c r="D30" s="3">
         <v>29</v>
       </c>
+      <c r="E30" s="2">
+        <v>1</v>
+      </c>
       <c r="F30" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
+      <c r="A31" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="15">
+        <v>42988</v>
+      </c>
       <c r="D31" s="2">
         <v>30</v>
       </c>
+      <c r="E31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" s="25" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
-      <c r="D32" s="3">
+      <c r="A32" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="15">
+        <v>42990</v>
+      </c>
+      <c r="D32" s="2">
         <v>31</v>
       </c>
+      <c r="E32" s="2">
+        <v>2</v>
+      </c>
+      <c r="F32" s="25" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
+      <c r="A33" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="15">
+        <v>42990</v>
+      </c>
       <c r="D33" s="2">
         <v>32</v>
       </c>
+      <c r="E33" s="2">
+        <v>1</v>
+      </c>
+      <c r="F33" s="25" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
-      <c r="D34" s="3">
+      <c r="A34" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="15">
+        <v>42990</v>
+      </c>
+      <c r="D34" s="2">
         <v>33</v>
       </c>
+      <c r="E34" s="2">
+        <v>1</v>
+      </c>
+      <c r="F34" s="25" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="19"/>
+      <c r="A35" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="15">
+        <v>42990</v>
+      </c>
+      <c r="C35" s="14"/>
       <c r="D35" s="2">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="E35" s="2">
+        <v>2</v>
+      </c>
+      <c r="F35" s="25" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
-      <c r="D36" s="3">
-        <v>35</v>
+      <c r="A36" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="15">
+        <v>42990</v>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="2">
+        <v>36</v>
+      </c>
+      <c r="E36" s="2">
+        <v>2</v>
+      </c>
+      <c r="F36" s="25" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
+      <c r="A37" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="15">
+        <v>42990</v>
+      </c>
+      <c r="C37" s="14"/>
       <c r="D37" s="2">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="E37" s="2">
+        <v>2</v>
+      </c>
+      <c r="F37" s="25" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
-      <c r="D38" s="3">
-        <v>37</v>
+      <c r="A38" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="15">
+        <v>42990</v>
+      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="2">
+        <v>38</v>
+      </c>
+      <c r="E38" s="2">
+        <v>2</v>
+      </c>
+      <c r="F38" s="25" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
+      <c r="A39" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="15">
+        <v>42990</v>
+      </c>
+      <c r="C39" s="14"/>
       <c r="D39" s="2">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="E39" s="2">
+        <v>2</v>
+      </c>
+      <c r="F39" s="25" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="21"/>
-      <c r="B40" s="16"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="3">
-        <v>39</v>
-      </c>
-      <c r="E40" s="5"/>
-      <c r="F40" s="24"/>
+      <c r="A40" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="15">
+        <v>42990</v>
+      </c>
+      <c r="C40" s="14"/>
+      <c r="D40" s="2">
+        <v>40</v>
+      </c>
+      <c r="E40" s="2">
+        <v>2</v>
+      </c>
+      <c r="F40" s="25" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="19"/>
-      <c r="D41" s="2">
-        <v>40</v>
+      <c r="A41" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="15">
+        <v>42990</v>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="3">
+        <v>41</v>
+      </c>
+      <c r="E41" s="2">
+        <v>2</v>
+      </c>
+      <c r="F41" s="25" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="19"/>
-      <c r="D42" s="3">
-        <v>41</v>
+      <c r="A42" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" s="15">
+        <v>42991</v>
+      </c>
+      <c r="D42" s="2">
+        <v>42</v>
+      </c>
+      <c r="E42" s="2">
+        <v>1</v>
+      </c>
+      <c r="F42" s="25" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="19"/>
-      <c r="D43" s="2">
-        <v>42</v>
+      <c r="A43" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="15">
+        <v>42991</v>
+      </c>
+      <c r="D43" s="3">
+        <v>43</v>
+      </c>
+      <c r="E43" s="2">
+        <v>1</v>
+      </c>
+      <c r="F43" s="25" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="19"/>
-      <c r="D44" s="3">
-        <v>43</v>
+      <c r="A44" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="15">
+        <v>42991</v>
+      </c>
+      <c r="D44" s="2">
+        <v>44</v>
+      </c>
+      <c r="E44" s="2">
+        <v>1</v>
+      </c>
+      <c r="F44" s="25" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="19"/>
-      <c r="D45" s="2">
-        <v>44</v>
+      <c r="A45" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="15">
+        <v>42991</v>
+      </c>
+      <c r="D45" s="3">
+        <v>45</v>
+      </c>
+      <c r="E45" s="2">
+        <v>1</v>
+      </c>
+      <c r="F45" s="25" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="19"/>
-      <c r="D46" s="3">
-        <v>45</v>
+      <c r="D46" s="2">
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="19"/>
-      <c r="D47" s="2">
-        <v>46</v>
+      <c r="D47" s="3">
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="19"/>
-      <c r="D48" s="3">
-        <v>47</v>
+      <c r="D48" s="2">
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="19"/>
-      <c r="D49" s="2">
-        <v>48</v>
+      <c r="D49" s="3">
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="19"/>
-      <c r="D50" s="3">
-        <v>49</v>
+      <c r="D50" s="2">
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="19"/>
-      <c r="D51" s="2">
-        <v>50</v>
+      <c r="D51" s="3">
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="19"/>
       <c r="B52" s="14"/>
-      <c r="D52" s="3">
-        <v>51</v>
+      <c r="D52" s="2">
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="19"/>
       <c r="B53" s="14"/>
-      <c r="D53" s="2">
-        <v>52</v>
+      <c r="D53" s="3">
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
-      <c r="D54" s="3">
-        <v>53</v>
+      <c r="D54" s="2">
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D55" s="2">
-        <v>54</v>
+      <c r="D55" s="3">
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D56" s="3">
-        <v>55</v>
+      <c r="D56" s="2">
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D57" s="2">
-        <v>56</v>
+      <c r="D57" s="3">
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D58" s="3">
-        <v>57</v>
+      <c r="D58" s="2">
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D59" s="2">
-        <v>58</v>
+      <c r="D59" s="3">
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D60" s="3">
-        <v>59</v>
+      <c r="D60" s="2">
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D61" s="2">
-        <v>60</v>
+      <c r="D61" s="3">
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D62" s="3">
-        <v>61</v>
+      <c r="D62" s="2">
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D63" s="2">
-        <v>62</v>
+      <c r="D63" s="3">
+        <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D64" s="3">
-        <v>63</v>
+      <c r="D64" s="2">
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D65" s="2">
-        <v>64</v>
+      <c r="D65" s="3">
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D66" s="3">
-        <v>65</v>
+      <c r="D66" s="2">
+        <v>66</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D67" s="2">
-        <v>66</v>
+      <c r="D67" s="3">
+        <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D68" s="3">
-        <v>67</v>
+      <c r="D68" s="2">
+        <v>68</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="21"/>
       <c r="B69" s="16"/>
       <c r="C69" s="16"/>
-      <c r="D69" s="2">
-        <v>68</v>
+      <c r="D69" s="3">
+        <v>69</v>
       </c>
       <c r="E69" s="5"/>
       <c r="F69" s="24"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D70" s="3">
-        <v>69</v>
+      <c r="D70" s="2">
+        <v>70</v>
       </c>
       <c r="G70" s="8"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D71" s="2">
-        <v>70</v>
+      <c r="D71" s="3">
+        <v>71</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D72" s="3">
-        <v>71</v>
+      <c r="D72" s="2">
+        <v>72</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D73" s="2">
-        <v>72</v>
+      <c r="D73" s="3">
+        <v>73</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D74" s="3">
-        <v>73</v>
+      <c r="D74" s="2">
+        <v>74</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D75" s="2">
-        <v>74</v>
+      <c r="D75" s="3">
+        <v>75</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D76" s="3">
-        <v>75</v>
+      <c r="D76" s="2">
+        <v>76</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D77" s="2">
-        <v>76</v>
+      <c r="D77" s="3">
+        <v>77</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D78" s="3">
-        <v>77</v>
+      <c r="D78" s="2">
+        <v>78</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="21"/>
       <c r="B79" s="16"/>
       <c r="C79" s="16"/>
-      <c r="D79" s="2">
-        <v>78</v>
+      <c r="D79" s="3">
+        <v>79</v>
       </c>
       <c r="E79" s="5"/>
       <c r="F79" s="24"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D80" s="3">
-        <v>79</v>
+      <c r="D80" s="2">
+        <v>80</v>
       </c>
     </row>
     <row r="81" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D81" s="2">
-        <v>80</v>
+      <c r="D81" s="3">
+        <v>81</v>
       </c>
     </row>
     <row r="82" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D82" s="3">
-        <v>81</v>
+      <c r="D82" s="2">
+        <v>82</v>
       </c>
     </row>
     <row r="83" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D83" s="2">
-        <v>82</v>
+      <c r="D83" s="3">
+        <v>83</v>
       </c>
     </row>
     <row r="84" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D84" s="3">
-        <v>83</v>
+      <c r="D84" s="2">
+        <v>84</v>
       </c>
     </row>
     <row r="85" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D85" s="2">
-        <v>84</v>
+      <c r="D85" s="3">
+        <v>85</v>
       </c>
     </row>
     <row r="86" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D86" s="3">
-        <v>85</v>
+      <c r="D86" s="2">
+        <v>86</v>
       </c>
     </row>
     <row r="87" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D87" s="2">
-        <v>86</v>
+      <c r="D87" s="3">
+        <v>87</v>
       </c>
     </row>
     <row r="88" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D88" s="3">
-        <v>87</v>
+      <c r="D88" s="2">
+        <v>88</v>
       </c>
     </row>
     <row r="89" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D89" s="2">
-        <v>88</v>
+      <c r="D89" s="3">
+        <v>89</v>
       </c>
     </row>
     <row r="90" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D90" s="3">
-        <v>89</v>
+      <c r="D90" s="2">
+        <v>90</v>
       </c>
     </row>
     <row r="91" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D91" s="2">
-        <v>90</v>
+      <c r="D91" s="3">
+        <v>91</v>
       </c>
     </row>
     <row r="92" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D92" s="3">
-        <v>91</v>
+      <c r="D92" s="2">
+        <v>92</v>
       </c>
     </row>
     <row r="93" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D93" s="2">
-        <v>92</v>
+      <c r="D93" s="3">
+        <v>93</v>
       </c>
     </row>
     <row r="94" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D94" s="3">
-        <v>93</v>
+      <c r="D94" s="2">
+        <v>94</v>
       </c>
     </row>
     <row r="95" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D95" s="2">
-        <v>94</v>
+      <c r="D95" s="3">
+        <v>95</v>
       </c>
     </row>
     <row r="96" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D96" s="3">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D97" s="2">
+      <c r="D96" s="2">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D98" s="3">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D97" s="3">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D99" s="2">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D98" s="2">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D100" s="3">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D99" s="3">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D101" s="2">
+    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D100" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B104" s="15">
-        <v>42988</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:G104"/>
+  <autoFilter ref="A1:G106"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
* implemended operator* * bugfix in operator+
</commit_message>
<xml_diff>
--- a/BIGNUM/Doc/bugs.xlsx
+++ b/BIGNUM/Doc/bugs.xlsx
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>Implementera Konstruktorn BigNumber(string)</t>
-  </si>
-  <si>
-    <t>Implementera BigNumber.operator+ Obs! För all aritmetik nedan gäller att om resultatet är negativt (-a), lagras (a) samt property Negative = true</t>
   </si>
   <si>
     <t>Implementera överlagrad konstruktor BigNumber(BigNumber num).</t>
@@ -152,9 +149,6 @@
     <t>Implementera operator &lt;= För BigNumber enbart</t>
   </si>
   <si>
-    <t>Implementera BigNumber.operator-. Unärt minus. Implementeras med hjälp av en flagga _negative. Let c = a-b . c &lt;  0  =&gt; lagra -(a-b) samt property Negative  = true.</t>
-  </si>
-  <si>
     <t>Implementera MakeEqual, som ser till att storleken på List&lt;uint&gt; _number är lika stor på bägge argumenten. Den största av operanderna får styra. För BigNumber enbart. Utgår. Man kan använda Trim() på de BigNumber som ingår i aritmetiken.Utgår eftersom numren har skapats via konstruktorer,  och då har de trimmats.</t>
   </si>
   <si>
@@ -198,9 +192,6 @@
   </si>
   <si>
     <t>Hårdoptimera för hastighet. Förallokera t.ex. listor om man vet deras storlek på förhand.</t>
-  </si>
-  <si>
-    <t>Korrigera datat från bas 10-strängarna till BASE-basen (dvs. den som inte var satt till 10 under testerna). Se BigNumber(string).</t>
   </si>
   <si>
     <t>Gå igenom alla Exceptions och kolla att rätt exception kastas vid rätt tillf älle</t>
@@ -245,16 +236,25 @@
     </r>
   </si>
   <si>
-    <t>Implementera /=</t>
-  </si>
-  <si>
-    <t>Implementera *=</t>
-  </si>
-  <si>
-    <t>Implementera -=</t>
-  </si>
-  <si>
-    <t>Implementera +=</t>
+    <t>Korrigera datat från bas 10-strängarna till BASE-basen (dvs. den som inte var satt till 10 under testerna). Se BigNumber(string). Samma som #28. Utgår.</t>
+  </si>
+  <si>
+    <t>Implementera /= Går antagligen inte att implementera, utan läggs ut av kompilatorn själv.</t>
+  </si>
+  <si>
+    <t>Implementera *= Går antagligen inte att implementera, utan läggs ut av kompilatorn själv.</t>
+  </si>
+  <si>
+    <t>Implementera += Går antagligen inte att implementera, utan läggs ut av kompilatorn själv.</t>
+  </si>
+  <si>
+    <t>Implementera -= Går antagligen inte att implementera, utan läggs ut av kompilatorn själv.</t>
+  </si>
+  <si>
+    <t>Implementera BigNumber.operator+ Obs! För all aritmetik gäller att om resultatet är negativt (-a), lagras (a) samt property Negative = true</t>
+  </si>
+  <si>
+    <t>Implementera BigNumber.operator-. Unärt minus.</t>
   </si>
 </sst>
 </file>
@@ -703,8 +703,8 @@
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E45" sqref="E45"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,8 +748,8 @@
       <c r="B2" s="14">
         <v>42981</v>
       </c>
-      <c r="C2" s="15">
-        <v>42987</v>
+      <c r="C2" s="14">
+        <v>42993</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
@@ -758,7 +758,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -778,17 +778,19 @@
         <v>1</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4" s="14">
         <v>42981</v>
       </c>
-      <c r="C4" s="14"/>
+      <c r="C4" s="14">
+        <v>42994</v>
+      </c>
       <c r="D4" s="3">
         <v>3</v>
       </c>
@@ -832,7 +834,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -847,10 +849,10 @@
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -870,7 +872,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -910,7 +912,7 @@
         <v>2</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -930,7 +932,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -950,7 +952,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G12" s="7"/>
     </row>
@@ -971,7 +973,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1008,7 +1010,7 @@
         <v>14</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F15" s="26" t="s">
         <v>15</v>
@@ -1031,7 +1033,7 @@
         <v>2</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1051,7 +1053,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1091,7 +1093,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1111,7 +1113,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1129,7 +1131,7 @@
         <v>2</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1149,7 +1151,7 @@
         <v>3</v>
       </c>
       <c r="F22" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1169,7 +1171,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1189,7 +1191,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1209,12 +1211,12 @@
         <v>1</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B26" s="17">
         <v>42988</v>
@@ -1227,7 +1229,7 @@
         <v>3</v>
       </c>
       <c r="F26" s="26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1247,7 +1249,7 @@
         <v>2</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1261,10 +1263,10 @@
         <v>27</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1278,15 +1280,15 @@
         <v>28</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B30" s="15">
         <v>42988</v>
@@ -1298,24 +1300,25 @@
         <v>1</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="15">
+      <c r="B31" s="16">
         <v>42988</v>
       </c>
-      <c r="D31" s="2">
+      <c r="C31" s="16"/>
+      <c r="D31" s="5">
         <v>30</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F31" s="25" t="s">
-        <v>42</v>
+      <c r="E31" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="24" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1332,7 +1335,7 @@
         <v>2</v>
       </c>
       <c r="F32" s="25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1349,7 +1352,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1366,7 +1369,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="25" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1384,7 +1387,7 @@
         <v>2</v>
       </c>
       <c r="F35" s="25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1402,7 +1405,7 @@
         <v>2</v>
       </c>
       <c r="F36" s="25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1420,7 +1423,7 @@
         <v>2</v>
       </c>
       <c r="F37" s="25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1438,7 +1441,7 @@
         <v>2</v>
       </c>
       <c r="F38" s="25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1456,7 +1459,7 @@
         <v>2</v>
       </c>
       <c r="F39" s="25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1474,7 +1477,7 @@
         <v>2</v>
       </c>
       <c r="F40" s="25" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1492,75 +1495,79 @@
         <v>2</v>
       </c>
       <c r="F41" s="25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" s="16">
+        <v>42991</v>
+      </c>
+      <c r="C42" s="16"/>
+      <c r="D42" s="5">
+        <v>42</v>
+      </c>
+      <c r="E42" s="5">
+        <v>1</v>
+      </c>
+      <c r="F42" s="24" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B42" s="15">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="16">
         <v>42991</v>
       </c>
-      <c r="D42" s="2">
-        <v>42</v>
-      </c>
-      <c r="E42" s="2">
-        <v>1</v>
-      </c>
-      <c r="F42" s="25" t="s">
+      <c r="C43" s="16"/>
+      <c r="D43" s="5">
+        <v>43</v>
+      </c>
+      <c r="E43" s="5">
+        <v>1</v>
+      </c>
+      <c r="F43" s="24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="16">
+        <v>42991</v>
+      </c>
+      <c r="C44" s="16"/>
+      <c r="D44" s="5">
+        <v>44</v>
+      </c>
+      <c r="E44" s="5">
+        <v>1</v>
+      </c>
+      <c r="F44" s="24" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="20" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B43" s="15">
+      <c r="B45" s="16">
         <v>42991</v>
       </c>
-      <c r="D43" s="3">
-        <v>43</v>
-      </c>
-      <c r="E43" s="2">
-        <v>1</v>
-      </c>
-      <c r="F43" s="25" t="s">
+      <c r="C45" s="16"/>
+      <c r="D45" s="5">
+        <v>45</v>
+      </c>
+      <c r="E45" s="5">
+        <v>1</v>
+      </c>
+      <c r="F45" s="24" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B44" s="15">
-        <v>42991</v>
-      </c>
-      <c r="D44" s="2">
-        <v>44</v>
-      </c>
-      <c r="E44" s="2">
-        <v>1</v>
-      </c>
-      <c r="F44" s="25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B45" s="15">
-        <v>42991</v>
-      </c>
-      <c r="D45" s="3">
-        <v>45</v>
-      </c>
-      <c r="E45" s="2">
-        <v>1</v>
-      </c>
-      <c r="F45" s="25" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added a reference to README.md
</commit_message>
<xml_diff>
--- a/BIGNUM/Doc/bugs.xlsx
+++ b/BIGNUM/Doc/bugs.xlsx
@@ -700,11 +700,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G100"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,7 +742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>5</v>
       </c>
@@ -761,7 +762,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>5</v>
       </c>
@@ -801,7 +802,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>11</v>
       </c>
@@ -837,7 +838,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>11</v>
       </c>
@@ -855,7 +856,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>7</v>
       </c>
@@ -875,7 +876,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>5</v>
       </c>
@@ -895,7 +896,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>5</v>
       </c>
@@ -915,7 +916,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>5</v>
       </c>
@@ -935,7 +936,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>5</v>
       </c>
@@ -956,7 +957,7 @@
       </c>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>5</v>
       </c>
@@ -976,7 +977,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>5</v>
       </c>
@@ -996,7 +997,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>5</v>
       </c>
@@ -1016,7 +1017,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>5</v>
       </c>
@@ -1036,7 +1037,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>5</v>
       </c>
@@ -1056,7 +1057,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>7</v>
       </c>
@@ -1076,7 +1077,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>7</v>
       </c>
@@ -1096,7 +1097,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>7</v>
       </c>
@@ -1134,7 +1135,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>5</v>
       </c>
@@ -1154,7 +1155,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>5</v>
       </c>
@@ -1174,7 +1175,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>7</v>
       </c>
@@ -1194,7 +1195,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>7</v>
       </c>
@@ -1214,7 +1215,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>34</v>
       </c>
@@ -1232,7 +1233,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>7</v>
       </c>
@@ -1252,7 +1253,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>11</v>
       </c>
@@ -1276,6 +1277,9 @@
       <c r="B29" s="15">
         <v>42988</v>
       </c>
+      <c r="C29" s="15">
+        <v>42994</v>
+      </c>
       <c r="D29" s="2">
         <v>28</v>
       </c>
@@ -1286,7 +1290,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>34</v>
       </c>
@@ -1321,7 +1325,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
         <v>11</v>
       </c>
@@ -1338,7 +1342,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>11</v>
       </c>
@@ -1355,7 +1359,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
         <v>11</v>
       </c>
@@ -1498,7 +1502,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
         <v>11</v>
       </c>
@@ -1570,134 +1574,134 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="19"/>
       <c r="D46" s="2">
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="19"/>
       <c r="D47" s="3">
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="19"/>
       <c r="D48" s="2">
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="19"/>
       <c r="D49" s="3">
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="19"/>
       <c r="D50" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="19"/>
       <c r="D51" s="3">
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="19"/>
       <c r="B52" s="14"/>
       <c r="D52" s="2">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="19"/>
       <c r="B53" s="14"/>
       <c r="D53" s="3">
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
       <c r="D54" s="2">
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D55" s="3">
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D56" s="2">
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D57" s="3">
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D58" s="2">
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D59" s="3">
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D60" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D61" s="3">
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D62" s="2">
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D63" s="3">
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D64" s="2">
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D65" s="3">
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D66" s="2">
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D67" s="3">
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D68" s="2">
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="21"/>
       <c r="B69" s="16"/>
       <c r="C69" s="16"/>
@@ -1707,53 +1711,53 @@
       <c r="E69" s="5"/>
       <c r="F69" s="24"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D70" s="2">
         <v>70</v>
       </c>
       <c r="G70" s="8"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D71" s="3">
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D72" s="2">
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D73" s="3">
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D74" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D75" s="3">
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D76" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D77" s="3">
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D78" s="2">
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="21"/>
       <c r="B79" s="16"/>
       <c r="C79" s="16"/>
@@ -1763,113 +1767,125 @@
       <c r="E79" s="5"/>
       <c r="F79" s="24"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D80" s="2">
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D81" s="3">
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D82" s="2">
         <v>82</v>
       </c>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D83" s="3">
         <v>83</v>
       </c>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D84" s="2">
         <v>84</v>
       </c>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D85" s="3">
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D86" s="2">
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D87" s="3">
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D88" s="2">
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D89" s="3">
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D90" s="2">
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D91" s="3">
         <v>91</v>
       </c>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D92" s="2">
         <v>92</v>
       </c>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D93" s="3">
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D94" s="2">
         <v>94</v>
       </c>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D95" s="3">
         <v>95</v>
       </c>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D96" s="2">
         <v>96</v>
       </c>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D97" s="3">
         <v>97</v>
       </c>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D98" s="2">
         <v>98</v>
       </c>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D99" s="3">
         <v>99</v>
       </c>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D100" s="2">
         <v>100</v>
       </c>
     </row>
+    <row r="101" spans="4:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="4:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="4:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="104" spans="4:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="4:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="4:4" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:G106"/>
+  <autoFilter ref="A1:G106">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="0.1.0.2"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>